<commit_message>
Restructure AWS and Azure LOE CSVs with proper SCOPE ASSUMPTIONS section
- AWS LOEs: Already had correct structure with Current Scope column
- Azure LOEs (4 solutions): Added complete SCOPE ASSUMPTIONS sections with:
  - Current Scope column (position 3, left of Small)
  - Solution-specific scope parameters
  - ESTIMATE SETTINGS with phase-based multipliers
  - EFFORT ESTIMATE section with Base Hours/Effort Multiplier/Actual Hours columns
- Regenerated all LOE Excel files with proper formatting:
  - Current Scope column highlighted with yellow background
  - Notes column width = 60 for better readability
  - All columns properly sized
</commit_message>
<xml_diff>
--- a/solutions/aws/ai/intelligent-document-processing/presales/level-of-effort-estimate.xlsx
+++ b/solutions/aws/ai/intelligent-document-processing/presales/level-of-effort-estimate.xlsx
@@ -13,7 +13,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LOE" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scope Assumptions'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Scope Assumptions'!$A$1:$E$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Scope Assumptions'!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -21,10 +22,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="$#,##0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="$#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,40 +35,56 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Segoe UI"/>
+      <color rgb="0095A5A6"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Segoe UI Light"/>
+      <color rgb="002C3E50"/>
+      <sz val="28"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <color rgb="005D6D7E"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
       <b val="1"/>
-      <color rgb="001F4E78"/>
-      <sz val="24"/>
+      <color rgb="005D6D7E"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <color rgb="0044546A"/>
-      <sz val="14"/>
+      <color rgb="002C3E50"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Segoe UI"/>
+      <color rgb="00CC0000"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <b val="1"/>
-      <color rgb="0044546A"/>
+      <color rgb="005D6D7E"/>
       <sz val="11"/>
+      <u val="single"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <color rgb="0044546A"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
+      <name val="Segoe UI Semibold"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
-      <color rgb="00000000"/>
+      <b val="1"/>
+      <color rgb="00CC0000"/>
       <sz val="12"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Segoe UI Semibold"/>
       <b val="1"/>
       <color rgb="00FFFFFF"/>
       <sz val="14"/>
@@ -77,7 +95,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -86,14 +104,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00808080"/>
-        <bgColor rgb="00808080"/>
+        <fgColor rgb="00CC0000"/>
+        <bgColor rgb="00CC0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F2F2F2"/>
-        <bgColor rgb="00F2F2F2"/>
+        <fgColor rgb="002C3E50"/>
+        <bgColor rgb="002C3E50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F8FAFB"/>
+        <bgColor rgb="00F8FAFB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E8F4F8"/>
+        <bgColor rgb="00E8F4F8"/>
       </patternFill>
     </fill>
     <fill>
@@ -104,18 +134,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00FFFFCC"/>
+        <bgColor rgb="00FFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00FFF2CC"/>
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00E8F4F8"/>
-        <bgColor rgb="00E8F4F8"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -124,54 +154,121 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color rgb="00BDC3C7"/>
+      </left>
+      <right style="thin">
+        <color rgb="00BDC3C7"/>
+      </right>
+      <top style="thin">
+        <color rgb="00BDC3C7"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="002C3E50"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00DEE2E6"/>
+      </left>
+      <right style="thin">
+        <color rgb="00DEE2E6"/>
+      </right>
+      <top style="thin">
+        <color rgb="00DEE2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00DEE2E6"/>
+      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -256,10 +353,10 @@
     <from>
       <col>1</col>
       <colOff>0</colOff>
-      <row>14</row>
+      <row>12</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="1143000" cy="285750"/>
+    <ext cx="1238250" cy="314325"/>
     <pic>
       <nvPicPr>
         <cNvPr id="1" name="Image 1" descr="Picture"/>
@@ -572,7 +669,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B4:C10"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,83 +677,107 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="5" customWidth="1" min="1" max="1"/>
-    <col width="30" customWidth="1" min="2" max="2"/>
-    <col width="13" customWidth="1" min="3" max="3"/>
-    <col width="5" customWidth="1" min="4" max="4"/>
+    <col width="3" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
+    <col width="3" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20" customHeight="1"/>
-    <row r="2" ht="10" customHeight="1"/>
-    <row r="3" ht="20" customHeight="1"/>
-    <row r="4" ht="30" customHeight="1">
-      <c r="B4" s="1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1">
+      <c r="B1" s="1" t="n"/>
+      <c r="C1" s="1" t="n"/>
+    </row>
+    <row r="2" ht="60" customHeight="1">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>[VENDOR LOGO]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1"/>
+    <row r="4" ht="40" customHeight="1">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Level Of Effort Estimate</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="20" customHeight="1">
-      <c r="B5" s="2" t="inlineStr">
+    <row r="5" ht="25" customHeight="1">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Presales Document</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="20" customHeight="1"/>
-    <row r="7">
-      <c r="B7" s="3" t="inlineStr">
+    <row r="6" ht="30" customHeight="1"/>
+    <row r="7" ht="18" customHeight="1">
+      <c r="B7" s="5" t="inlineStr">
         <is>
           <t>Generated:</t>
         </is>
       </c>
-      <c r="C7" s="4" t="inlineStr">
-        <is>
-          <t>November 15, 2025</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="3" t="inlineStr">
+      <c r="C7" s="6" t="inlineStr">
+        <is>
+          <t>November 16, 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="B8" s="5" t="inlineStr">
         <is>
           <t>Solution:</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="6" t="inlineStr">
         <is>
           <t>Intelligent Document Processing</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>Customer Name:</t>
-        </is>
-      </c>
-      <c r="C9" s="4" t="inlineStr">
+    <row r="9" ht="18" customHeight="1">
+      <c r="B9" s="5" t="inlineStr">
+        <is>
+          <t>Customer:</t>
+        </is>
+      </c>
+      <c r="C9" s="6" t="inlineStr">
         <is>
           <t>[Customer Name]</t>
         </is>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="3" t="inlineStr">
+    <row r="10" ht="18" customHeight="1">
+      <c r="B10" s="5" t="inlineStr">
         <is>
           <t>Version:</t>
         </is>
       </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>1.0</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="20" customHeight="1"/>
-    <row r="12" ht="10" customHeight="1"/>
-    <row r="13" ht="10" customHeight="1"/>
-    <row r="14" ht="10" customHeight="1"/>
-    <row r="15" ht="40" customHeight="1"/>
+    <row r="11" ht="18" customHeight="1">
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>Status:</t>
+        </is>
+      </c>
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Draft</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="40" customHeight="1"/>
+    <row r="13" ht="30" customHeight="1">
+      <c r="C13" s="8" t="inlineStr">
+        <is>
+          <t>eoframework.org</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -667,9 +788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -680,657 +801,744 @@
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
     <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="30" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="25" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="60" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="19" t="inlineStr">
         <is>
           <t>Baseline Assumption</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="19" t="inlineStr">
+        <is>
+          <t>Current Scope</t>
+        </is>
+      </c>
+      <c r="D1" s="19" t="inlineStr">
         <is>
           <t>Small (1x)</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="E1" s="19" t="inlineStr">
         <is>
           <t>Medium (2x)</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="F1" s="19" t="inlineStr">
         <is>
           <t>Large (3x)</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="G1" s="19" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr"/>
-      <c r="H1" s="5" t="inlineStr"/>
-      <c r="I1" s="5" t="inlineStr"/>
-      <c r="J1" s="5" t="inlineStr"/>
-      <c r="K1" s="5" t="inlineStr"/>
+      <c r="H1" s="19" t="inlineStr"/>
+      <c r="I1" s="19" t="inlineStr"/>
+      <c r="J1" s="19" t="inlineStr"/>
+      <c r="K1" s="19" t="inlineStr"/>
+      <c r="L1" s="19" t="inlineStr"/>
     </row>
     <row r="2" ht="26" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>Solution Scope</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="10" t="inlineStr">
         <is>
           <t>Document Types</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="20" t="inlineStr">
         <is>
           <t>2-3 document types</t>
         </is>
       </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="D2" s="10" t="inlineStr">
+        <is>
+          <t>2-3 document types</t>
+        </is>
+      </c>
+      <c r="E2" s="10" t="inlineStr">
         <is>
           <t>4-6 document types</t>
         </is>
       </c>
-      <c r="E2" s="6" t="inlineStr">
+      <c r="F2" s="10" t="inlineStr">
         <is>
           <t>8+ document types or complex variations</t>
         </is>
       </c>
-      <c r="F2" s="6" t="inlineStr">
+      <c r="G2" s="10" t="inlineStr">
         <is>
           <t>Standard document types for IDP</t>
         </is>
       </c>
-      <c r="G2" s="6" t="inlineStr"/>
-      <c r="H2" s="6" t="inlineStr"/>
-      <c r="I2" s="6" t="inlineStr"/>
-      <c r="J2" s="6" t="inlineStr"/>
-      <c r="K2" s="6" t="inlineStr"/>
+      <c r="H2" s="10" t="inlineStr"/>
+      <c r="I2" s="10" t="inlineStr"/>
+      <c r="J2" s="10" t="inlineStr"/>
+      <c r="K2" s="10" t="inlineStr"/>
+      <c r="L2" s="10" t="inlineStr"/>
     </row>
     <row r="3" ht="26" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="21" t="inlineStr">
         <is>
           <t>Solution Scope</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="21" t="inlineStr">
         <is>
           <t>AI/ML Complexity</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="20" t="inlineStr">
         <is>
           <t>AWS Textract/Comprehend only</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="21" t="inlineStr">
+        <is>
+          <t>AWS Textract/Comprehend only</t>
+        </is>
+      </c>
+      <c r="E3" s="21" t="inlineStr">
         <is>
           <t>Custom classification models</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
+      <c r="F3" s="21" t="inlineStr">
         <is>
           <t>Advanced custom models + NLP</t>
         </is>
       </c>
-      <c r="F3" s="7" t="inlineStr">
+      <c r="G3" s="21" t="inlineStr">
         <is>
           <t>Pre-built vs custom model development</t>
         </is>
       </c>
-      <c r="G3" s="7" t="inlineStr"/>
-      <c r="H3" s="7" t="inlineStr"/>
-      <c r="I3" s="7" t="inlineStr"/>
-      <c r="J3" s="7" t="inlineStr"/>
-      <c r="K3" s="7" t="inlineStr"/>
+      <c r="H3" s="21" t="inlineStr"/>
+      <c r="I3" s="21" t="inlineStr"/>
+      <c r="J3" s="21" t="inlineStr"/>
+      <c r="K3" s="21" t="inlineStr"/>
+      <c r="L3" s="21" t="inlineStr"/>
     </row>
     <row r="4" ht="26" customHeight="1">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>External System Integrations</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="20" t="inlineStr">
         <is>
           <t>2 REST APIs</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="10" t="inlineStr">
+        <is>
+          <t>2 REST APIs</t>
+        </is>
+      </c>
+      <c r="E4" s="10" t="inlineStr">
         <is>
           <t>4-6 systems</t>
         </is>
       </c>
-      <c r="E4" s="6" t="inlineStr">
+      <c r="F4" s="10" t="inlineStr">
         <is>
           <t>8+ systems or complex protocols</t>
         </is>
       </c>
-      <c r="F4" s="6" t="inlineStr">
+      <c r="G4" s="10" t="inlineStr">
         <is>
           <t>Standard REST/API integrations for document flow</t>
         </is>
       </c>
-      <c r="G4" s="6" t="inlineStr"/>
-      <c r="H4" s="6" t="inlineStr"/>
-      <c r="I4" s="6" t="inlineStr"/>
-      <c r="J4" s="6" t="inlineStr"/>
-      <c r="K4" s="6" t="inlineStr"/>
+      <c r="H4" s="10" t="inlineStr"/>
+      <c r="I4" s="10" t="inlineStr"/>
+      <c r="J4" s="10" t="inlineStr"/>
+      <c r="K4" s="10" t="inlineStr"/>
+      <c r="L4" s="10" t="inlineStr"/>
     </row>
     <row r="5" ht="26" customHeight="1">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="21" t="inlineStr">
         <is>
           <t>Integration</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="21" t="inlineStr">
         <is>
           <t>Data Sources</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="20" t="inlineStr">
+        <is>
+          <t>S3 and email ingestion</t>
+        </is>
+      </c>
+      <c r="D5" s="21" t="inlineStr">
         <is>
           <t>2-3 data sources</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="E5" s="21" t="inlineStr">
         <is>
           <t>4-6 data sources</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
+      <c r="F5" s="21" t="inlineStr">
         <is>
           <t>8+ data sources or complex formats</t>
         </is>
       </c>
-      <c r="F5" s="7" t="inlineStr">
+      <c r="G5" s="21" t="inlineStr">
         <is>
           <t>Document input channels and storage</t>
         </is>
       </c>
-      <c r="G5" s="7" t="inlineStr"/>
-      <c r="H5" s="7" t="inlineStr"/>
-      <c r="I5" s="7" t="inlineStr"/>
-      <c r="J5" s="7" t="inlineStr"/>
-      <c r="K5" s="7" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="H5" s="21" t="inlineStr"/>
+      <c r="I5" s="21" t="inlineStr"/>
+      <c r="J5" s="21" t="inlineStr"/>
+      <c r="K5" s="21" t="inlineStr"/>
+      <c r="L5" s="21" t="inlineStr"/>
+    </row>
+    <row r="6" ht="26" customHeight="1">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>User Base</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>Total Users</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" s="20" t="inlineStr">
         <is>
           <t>50 users</t>
         </is>
       </c>
-      <c r="D6" s="6" t="inlineStr">
+      <c r="D6" s="10" t="inlineStr">
+        <is>
+          <t>50 users</t>
+        </is>
+      </c>
+      <c r="E6" s="10" t="inlineStr">
         <is>
           <t>100-250 users</t>
         </is>
       </c>
-      <c r="E6" s="6" t="inlineStr">
+      <c r="F6" s="10" t="inlineStr">
         <is>
           <t>500+ users</t>
         </is>
       </c>
-      <c r="F6" s="6" t="inlineStr">
+      <c r="G6" s="10" t="inlineStr">
         <is>
           <t>Users submitting and reviewing documents</t>
         </is>
       </c>
-      <c r="G6" s="6" t="inlineStr"/>
-      <c r="H6" s="6" t="inlineStr"/>
-      <c r="I6" s="6" t="inlineStr"/>
-      <c r="J6" s="6" t="inlineStr"/>
-      <c r="K6" s="6" t="inlineStr"/>
+      <c r="H6" s="10" t="inlineStr"/>
+      <c r="I6" s="10" t="inlineStr"/>
+      <c r="J6" s="10" t="inlineStr"/>
+      <c r="K6" s="10" t="inlineStr"/>
+      <c r="L6" s="10" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="21" t="inlineStr">
         <is>
           <t>User Base</t>
         </is>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="21" t="inlineStr">
         <is>
           <t>User Roles</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="20" t="inlineStr">
+        <is>
+          <t>3 roles (submitter reviewer admin)</t>
+        </is>
+      </c>
+      <c r="D7" s="21" t="inlineStr">
         <is>
           <t>2-3 standard roles</t>
         </is>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="E7" s="21" t="inlineStr">
         <is>
           <t>4-6 roles</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="F7" s="21" t="inlineStr">
         <is>
           <t>8+ roles with complex permissions</t>
         </is>
       </c>
-      <c r="F7" s="7" t="inlineStr">
+      <c r="G7" s="21" t="inlineStr">
         <is>
           <t>Document processors reviewers administrators</t>
         </is>
       </c>
-      <c r="G7" s="7" t="inlineStr"/>
-      <c r="H7" s="7" t="inlineStr"/>
-      <c r="I7" s="7" t="inlineStr"/>
-      <c r="J7" s="7" t="inlineStr"/>
-      <c r="K7" s="7" t="inlineStr"/>
+      <c r="H7" s="21" t="inlineStr"/>
+      <c r="I7" s="21" t="inlineStr"/>
+      <c r="J7" s="21" t="inlineStr"/>
+      <c r="K7" s="21" t="inlineStr"/>
+      <c r="L7" s="21" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Data Volume</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>Document Processing Volume</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="20" t="inlineStr">
         <is>
           <t>1000-5000 docs/month</t>
         </is>
       </c>
-      <c r="D8" s="6" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
+        <is>
+          <t>1000-5000 docs/month</t>
+        </is>
+      </c>
+      <c r="E8" s="10" t="inlineStr">
         <is>
           <t>10000-50000 docs/month</t>
         </is>
       </c>
-      <c r="E8" s="6" t="inlineStr">
+      <c r="F8" s="10" t="inlineStr">
         <is>
           <t>100000+ docs/month</t>
         </is>
       </c>
-      <c r="F8" s="6" t="inlineStr">
+      <c r="G8" s="10" t="inlineStr">
         <is>
           <t>Monthly document processing volume</t>
         </is>
       </c>
-      <c r="G8" s="6" t="inlineStr"/>
-      <c r="H8" s="6" t="inlineStr"/>
-      <c r="I8" s="6" t="inlineStr"/>
-      <c r="J8" s="6" t="inlineStr"/>
-      <c r="K8" s="6" t="inlineStr"/>
+      <c r="H8" s="10" t="inlineStr"/>
+      <c r="I8" s="10" t="inlineStr"/>
+      <c r="J8" s="10" t="inlineStr"/>
+      <c r="K8" s="10" t="inlineStr"/>
+      <c r="L8" s="10" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Data Volume</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="21" t="inlineStr">
         <is>
           <t>Data Storage Requirements</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr">
+      <c r="C9" s="20" t="inlineStr">
         <is>
           <t>500 GB</t>
         </is>
       </c>
-      <c r="D9" s="7" t="inlineStr">
+      <c r="D9" s="21" t="inlineStr">
+        <is>
+          <t>500 GB</t>
+        </is>
+      </c>
+      <c r="E9" s="21" t="inlineStr">
         <is>
           <t>2 TB</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
+      <c r="F9" s="21" t="inlineStr">
         <is>
           <t>10+ TB</t>
         </is>
       </c>
-      <c r="F9" s="7" t="inlineStr">
+      <c r="G9" s="21" t="inlineStr">
         <is>
           <t>Document storage and retention</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
-      <c r="H9" s="7" t="inlineStr"/>
-      <c r="I9" s="7" t="inlineStr"/>
-      <c r="J9" s="7" t="inlineStr"/>
-      <c r="K9" s="7" t="inlineStr"/>
+      <c r="H9" s="21" t="inlineStr"/>
+      <c r="I9" s="21" t="inlineStr"/>
+      <c r="J9" s="21" t="inlineStr"/>
+      <c r="K9" s="21" t="inlineStr"/>
+      <c r="L9" s="21" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>Technical Environment</t>
         </is>
       </c>
-      <c r="B10" s="6" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>Deployment Regions</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C10" s="20" t="inlineStr">
+        <is>
+          <t>Single AWS region (us-east-1)</t>
+        </is>
+      </c>
+      <c r="D10" s="10" t="inlineStr">
         <is>
           <t>Single AWS region</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
+      <c r="E10" s="10" t="inlineStr">
         <is>
           <t>2-3 regions</t>
         </is>
       </c>
-      <c r="E10" s="6" t="inlineStr">
+      <c r="F10" s="10" t="inlineStr">
         <is>
           <t>Global multi-region</t>
         </is>
       </c>
-      <c r="F10" s="6" t="inlineStr">
+      <c r="G10" s="10" t="inlineStr">
         <is>
           <t>Geographic distribution for IDP</t>
         </is>
       </c>
-      <c r="G10" s="6" t="inlineStr"/>
-      <c r="H10" s="6" t="inlineStr"/>
-      <c r="I10" s="6" t="inlineStr"/>
-      <c r="J10" s="6" t="inlineStr"/>
-      <c r="K10" s="6" t="inlineStr"/>
+      <c r="H10" s="10" t="inlineStr"/>
+      <c r="I10" s="10" t="inlineStr"/>
+      <c r="J10" s="10" t="inlineStr"/>
+      <c r="K10" s="10" t="inlineStr"/>
+      <c r="L10" s="10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="21" t="inlineStr">
         <is>
           <t>Technical Environment</t>
         </is>
       </c>
-      <c r="B11" s="7" t="inlineStr">
+      <c r="B11" s="21" t="inlineStr">
         <is>
           <t>Availability Requirements</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr">
+      <c r="C11" s="20" t="inlineStr">
         <is>
           <t>Standard (99.5%)</t>
         </is>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="21" t="inlineStr">
+        <is>
+          <t>Standard (99.5%)</t>
+        </is>
+      </c>
+      <c r="E11" s="21" t="inlineStr">
         <is>
           <t>High availability (99.9%)</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
+      <c r="F11" s="21" t="inlineStr">
         <is>
           <t>Mission critical (99.95%+)</t>
         </is>
       </c>
-      <c r="F11" s="7" t="inlineStr">
+      <c r="G11" s="21" t="inlineStr">
         <is>
           <t>SLA for document processing</t>
         </is>
       </c>
-      <c r="G11" s="7" t="inlineStr"/>
-      <c r="H11" s="7" t="inlineStr"/>
-      <c r="I11" s="7" t="inlineStr"/>
-      <c r="J11" s="7" t="inlineStr"/>
-      <c r="K11" s="7" t="inlineStr"/>
+      <c r="H11" s="21" t="inlineStr"/>
+      <c r="I11" s="21" t="inlineStr"/>
+      <c r="J11" s="21" t="inlineStr"/>
+      <c r="K11" s="21" t="inlineStr"/>
+      <c r="L11" s="21" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Technical Environment</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" s="10" t="inlineStr">
         <is>
           <t>Infrastructure Complexity</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
+      <c r="C12" s="20" t="inlineStr">
+        <is>
+          <t>Serverless (Lambda S3 Textract)</t>
+        </is>
+      </c>
+      <c r="D12" s="10" t="inlineStr">
         <is>
           <t>Basic serverless</t>
         </is>
       </c>
-      <c r="D12" s="6" t="inlineStr">
+      <c r="E12" s="10" t="inlineStr">
         <is>
           <t>Multi-tier standard</t>
         </is>
       </c>
-      <c r="E12" s="6" t="inlineStr">
+      <c r="F12" s="10" t="inlineStr">
         <is>
           <t>Complex distributed with custom ML</t>
         </is>
       </c>
-      <c r="F12" s="6" t="inlineStr">
+      <c r="G12" s="10" t="inlineStr">
         <is>
           <t>AWS Lambda S3 Textract Comprehend architecture</t>
         </is>
       </c>
-      <c r="G12" s="6" t="inlineStr"/>
-      <c r="H12" s="6" t="inlineStr"/>
-      <c r="I12" s="6" t="inlineStr"/>
-      <c r="J12" s="6" t="inlineStr"/>
-      <c r="K12" s="6" t="inlineStr"/>
+      <c r="H12" s="10" t="inlineStr"/>
+      <c r="I12" s="10" t="inlineStr"/>
+      <c r="J12" s="10" t="inlineStr"/>
+      <c r="K12" s="10" t="inlineStr"/>
+      <c r="L12" s="10" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="21" t="inlineStr">
         <is>
           <t>Security &amp; Compliance</t>
         </is>
       </c>
-      <c r="B13" s="7" t="inlineStr">
+      <c r="B13" s="21" t="inlineStr">
         <is>
           <t>Security Requirements</t>
         </is>
       </c>
-      <c r="C13" s="7" t="inlineStr">
+      <c r="C13" s="20" t="inlineStr">
+        <is>
+          <t>Basic encryption IAM SSE-S3</t>
+        </is>
+      </c>
+      <c r="D13" s="21" t="inlineStr">
         <is>
           <t>Basic encryption IAM</t>
         </is>
       </c>
-      <c r="D13" s="7" t="inlineStr">
+      <c r="E13" s="21" t="inlineStr">
         <is>
           <t>Industry standard (SOC2 HIPAA)</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
+      <c r="F13" s="21" t="inlineStr">
         <is>
           <t>Advanced (FedRAMP multi-jurisdiction)</t>
         </is>
       </c>
-      <c r="F13" s="7" t="inlineStr">
+      <c r="G13" s="21" t="inlineStr">
         <is>
           <t>Document security and access controls</t>
         </is>
       </c>
-      <c r="G13" s="7" t="inlineStr"/>
-      <c r="H13" s="7" t="inlineStr"/>
-      <c r="I13" s="7" t="inlineStr"/>
-      <c r="J13" s="7" t="inlineStr"/>
-      <c r="K13" s="7" t="inlineStr"/>
+      <c r="H13" s="21" t="inlineStr"/>
+      <c r="I13" s="21" t="inlineStr"/>
+      <c r="J13" s="21" t="inlineStr"/>
+      <c r="K13" s="21" t="inlineStr"/>
+      <c r="L13" s="21" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Security &amp; Compliance</t>
         </is>
       </c>
-      <c r="B14" s="6" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>Compliance Frameworks</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
+      <c r="C14" s="20" t="inlineStr">
+        <is>
+          <t>SOC2</t>
+        </is>
+      </c>
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>1-2 basic standards</t>
         </is>
       </c>
-      <c r="D14" s="6" t="inlineStr">
+      <c r="E14" s="10" t="inlineStr">
         <is>
           <t>2-3 industry standards</t>
         </is>
       </c>
-      <c r="E14" s="6" t="inlineStr">
+      <c r="F14" s="10" t="inlineStr">
         <is>
           <t>Multiple complex frameworks</t>
         </is>
       </c>
-      <c r="F14" s="6" t="inlineStr">
+      <c r="G14" s="10" t="inlineStr">
         <is>
           <t>Regulatory compliance for documents</t>
         </is>
       </c>
-      <c r="G14" s="6" t="inlineStr"/>
-      <c r="H14" s="6" t="inlineStr"/>
-      <c r="I14" s="6" t="inlineStr"/>
-      <c r="J14" s="6" t="inlineStr"/>
-      <c r="K14" s="6" t="inlineStr"/>
+      <c r="H14" s="10" t="inlineStr"/>
+      <c r="I14" s="10" t="inlineStr"/>
+      <c r="J14" s="10" t="inlineStr"/>
+      <c r="K14" s="10" t="inlineStr"/>
+      <c r="L14" s="10" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="A15" s="21" t="inlineStr">
         <is>
           <t>Performance</t>
         </is>
       </c>
-      <c r="B15" s="7" t="inlineStr">
+      <c r="B15" s="21" t="inlineStr">
         <is>
           <t>Accuracy Requirements</t>
         </is>
       </c>
-      <c r="C15" s="7" t="inlineStr">
+      <c r="C15" s="20" t="inlineStr">
+        <is>
+          <t>95%+ extraction accuracy</t>
+        </is>
+      </c>
+      <c r="D15" s="21" t="inlineStr">
         <is>
           <t>95%+ standard</t>
         </is>
       </c>
-      <c r="D15" s="7" t="inlineStr">
+      <c r="E15" s="21" t="inlineStr">
         <is>
           <t>98%+ enhanced</t>
         </is>
       </c>
-      <c r="E15" s="7" t="inlineStr">
+      <c r="F15" s="21" t="inlineStr">
         <is>
           <t>99%+ with human review</t>
         </is>
       </c>
-      <c r="F15" s="7" t="inlineStr">
+      <c r="G15" s="21" t="inlineStr">
         <is>
           <t>Data extraction accuracy targets</t>
         </is>
       </c>
-      <c r="G15" s="7" t="inlineStr"/>
-      <c r="H15" s="7" t="inlineStr"/>
-      <c r="I15" s="7" t="inlineStr"/>
-      <c r="J15" s="7" t="inlineStr"/>
-      <c r="K15" s="7" t="inlineStr"/>
+      <c r="H15" s="21" t="inlineStr"/>
+      <c r="I15" s="21" t="inlineStr"/>
+      <c r="J15" s="21" t="inlineStr"/>
+      <c r="K15" s="21" t="inlineStr"/>
+      <c r="L15" s="21" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>Performance</t>
         </is>
       </c>
-      <c r="B16" s="6" t="inlineStr">
+      <c r="B16" s="10" t="inlineStr">
         <is>
           <t>Processing Speed</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
+      <c r="C16" s="20" t="inlineStr">
         <is>
           <t>Standard batch processing</t>
         </is>
       </c>
-      <c r="D16" s="6" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Standard batch processing</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr">
         <is>
           <t>Near real-time processing</t>
         </is>
       </c>
-      <c r="E16" s="6" t="inlineStr">
+      <c r="F16" s="10" t="inlineStr">
         <is>
           <t>Real-time with sub-second response</t>
         </is>
       </c>
-      <c r="F16" s="6" t="inlineStr">
+      <c r="G16" s="10" t="inlineStr">
         <is>
           <t>Document processing speed requirements</t>
         </is>
       </c>
-      <c r="G16" s="6" t="inlineStr"/>
-      <c r="H16" s="6" t="inlineStr"/>
-      <c r="I16" s="6" t="inlineStr"/>
-      <c r="J16" s="6" t="inlineStr"/>
-      <c r="K16" s="6" t="inlineStr"/>
+      <c r="H16" s="10" t="inlineStr"/>
+      <c r="I16" s="10" t="inlineStr"/>
+      <c r="J16" s="10" t="inlineStr"/>
+      <c r="K16" s="10" t="inlineStr"/>
+      <c r="L16" s="10" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="A17" s="21" t="inlineStr">
         <is>
           <t>Environment</t>
         </is>
       </c>
-      <c r="B17" s="7" t="inlineStr">
+      <c r="B17" s="21" t="inlineStr">
         <is>
           <t>Deployment Environments</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
+      <c r="C17" s="20" t="inlineStr">
         <is>
           <t>2 environments (dev prod)</t>
         </is>
       </c>
-      <c r="D17" s="7" t="inlineStr">
+      <c r="D17" s="21" t="inlineStr">
+        <is>
+          <t>2 environments (dev prod)</t>
+        </is>
+      </c>
+      <c r="E17" s="21" t="inlineStr">
         <is>
           <t>3 environments (dev staging prod)</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="F17" s="21" t="inlineStr">
         <is>
           <t>4+ environments with ML pipelines</t>
         </is>
       </c>
-      <c r="F17" s="7" t="inlineStr">
+      <c r="G17" s="21" t="inlineStr">
         <is>
           <t>Environment management for IDP</t>
         </is>
       </c>
-      <c r="G17" s="7" t="inlineStr"/>
-      <c r="H17" s="7" t="inlineStr"/>
-      <c r="I17" s="7" t="inlineStr"/>
-      <c r="J17" s="7" t="inlineStr"/>
-      <c r="K17" s="7" t="inlineStr"/>
+      <c r="H17" s="21" t="inlineStr"/>
+      <c r="I17" s="21" t="inlineStr"/>
+      <c r="J17" s="21" t="inlineStr"/>
+      <c r="K17" s="21" t="inlineStr"/>
+      <c r="L17" s="21" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="inlineStr"/>
-      <c r="B18" s="6" t="inlineStr"/>
-      <c r="C18" s="6" t="inlineStr"/>
-      <c r="D18" s="6" t="inlineStr"/>
-      <c r="E18" s="6" t="inlineStr"/>
-      <c r="F18" s="6" t="inlineStr"/>
-      <c r="G18" s="6" t="inlineStr"/>
-      <c r="H18" s="6" t="inlineStr"/>
-      <c r="I18" s="6" t="inlineStr"/>
-      <c r="J18" s="6" t="inlineStr"/>
-      <c r="K18" s="6" t="inlineStr"/>
+      <c r="A18" s="10" t="inlineStr"/>
+      <c r="B18" s="10" t="inlineStr"/>
+      <c r="C18" s="10" t="inlineStr"/>
+      <c r="D18" s="10" t="inlineStr"/>
+      <c r="E18" s="10" t="inlineStr"/>
+      <c r="F18" s="10" t="inlineStr"/>
+      <c r="G18" s="10" t="inlineStr"/>
+      <c r="H18" s="10" t="inlineStr"/>
+      <c r="I18" s="10" t="inlineStr"/>
+      <c r="J18" s="10" t="inlineStr"/>
+      <c r="K18" s="10" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <autoFilter ref="A1:E6"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" fitToHeight="0" fitToWidth="1"/>
 </worksheet>
 </file>
 
@@ -1355,423 +1563,423 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="22" t="inlineStr">
         <is>
           <t>INSTRUCTIONS: How to Use Estimate Settings</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="9" t="inlineStr"/>
+      <c r="A2" s="23" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="inlineStr">
+      <c r="A3" s="23" t="inlineStr">
         <is>
           <t>This sheet contains phase-based multiplier variables that control effort scaling for each project phase.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="inlineStr">
+      <c r="A4" s="23" t="inlineStr">
         <is>
           <t>The EO Sales Engineer updates these multipliers based on customer scope compared to baseline assumptions.</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="9" t="inlineStr"/>
+      <c r="A5" s="23" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="A6" s="24" t="inlineStr">
         <is>
           <t>How It Works:</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="9" t="inlineStr">
+      <c r="A7" s="23" t="inlineStr">
         <is>
           <t>1. Review customer requirements from Discovery Questionnaire</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="9" t="inlineStr">
+      <c r="A8" s="23" t="inlineStr">
         <is>
           <t>2. Compare customer scope to Baseline Assumptions (see 'Scope Assumptions' sheet)</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="inlineStr">
+      <c r="A9" s="23" t="inlineStr">
         <is>
           <t>3. Update YELLOW HIGHLIGHTED multiplier values below (Column C) for each phase</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="9" t="inlineStr">
+      <c r="A10" s="23" t="inlineStr">
         <is>
           <t>4. All tasks in that phase on the 'LOE' sheet automatically update their Actual Hours</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="9" t="inlineStr">
+      <c r="A11" s="23" t="inlineStr">
         <is>
           <t>5. Total cost recalculates automatically</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9" t="inlineStr"/>
+      <c r="A12" s="23" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="inlineStr">
+      <c r="A13" s="24" t="inlineStr">
         <is>
           <t>Multiplier Guidelines:</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="9" t="inlineStr">
+      <c r="A14" s="23" t="inlineStr">
         <is>
           <t>• 1.0 = Matches baseline exactly (Small scope)</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="9" t="inlineStr">
+      <c r="A15" s="23" t="inlineStr">
         <is>
           <t>• 1.5-2.0 = Medium scope (moderately above baseline)</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="9" t="inlineStr">
+      <c r="A16" s="23" t="inlineStr">
         <is>
           <t>• 2.0-3.0 = Large scope (significantly above baseline)</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="9" t="inlineStr">
+      <c r="A17" s="23" t="inlineStr">
         <is>
           <t>• 3.0+ = Very large/complex (substantially above baseline, document rationale)</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="9" t="inlineStr"/>
+      <c r="A18" s="23" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="9" t="inlineStr">
+      <c r="A19" s="23" t="inlineStr">
         <is>
           <t>Example: Customer needs comprehensive testing due to compliance → Set TESTING_MX to 2.0</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="9" t="inlineStr">
+      <c r="A20" s="23" t="inlineStr">
         <is>
           <t>Example: Complex architecture requiring more technical oversight → Set LEADERSHIP_MX to 1.5</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="9" t="inlineStr"/>
+      <c r="A21" s="23" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="inlineStr">
+      <c r="A22" s="25" t="inlineStr">
         <is>
           <t>ESTIMATE SETTINGS - Update phase multipliers in Column C below:</t>
         </is>
       </c>
     </row>
     <row r="23" ht="32" customHeight="1">
-      <c r="A23" s="5" t="inlineStr">
+      <c r="A23" s="19" t="inlineStr">
         <is>
           <t>Phase</t>
         </is>
       </c>
-      <c r="B23" s="5" t="inlineStr">
+      <c r="B23" s="19" t="inlineStr">
         <is>
           <t>Variable Name</t>
         </is>
       </c>
-      <c r="C23" s="5" t="inlineStr">
+      <c r="C23" s="19" t="inlineStr">
         <is>
           <t>Multiplier</t>
         </is>
       </c>
-      <c r="D23" s="5" t="inlineStr">
+      <c r="D23" s="19" t="inlineStr">
         <is>
           <t>Description / Applies To Tasks</t>
         </is>
       </c>
-      <c r="E23" s="5" t="inlineStr"/>
-      <c r="F23" s="5" t="inlineStr"/>
-      <c r="G23" s="5" t="inlineStr"/>
-      <c r="H23" s="5" t="inlineStr"/>
-      <c r="I23" s="5" t="inlineStr"/>
-      <c r="J23" s="5" t="inlineStr"/>
-      <c r="K23" s="5" t="inlineStr"/>
+      <c r="E23" s="19" t="inlineStr"/>
+      <c r="F23" s="19" t="inlineStr"/>
+      <c r="G23" s="19" t="inlineStr"/>
+      <c r="H23" s="19" t="inlineStr"/>
+      <c r="I23" s="19" t="inlineStr"/>
+      <c r="J23" s="19" t="inlineStr"/>
+      <c r="K23" s="19" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="inlineStr">
+      <c r="A24" s="10" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="B24" s="6" t="inlineStr">
+      <c r="B24" s="10" t="inlineStr">
         <is>
           <t>DISCOVERY_MX</t>
         </is>
       </c>
-      <c r="C24" s="12" t="n">
+      <c r="C24" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D24" s="6" t="inlineStr">
+      <c r="D24" s="10" t="inlineStr">
         <is>
           <t>All Discovery phase tasks (Requirements Gathering, Document Analysis, AWS Assessment, Compliance Review)</t>
         </is>
       </c>
-      <c r="E24" s="6" t="inlineStr"/>
-      <c r="F24" s="6" t="inlineStr"/>
-      <c r="G24" s="6" t="inlineStr"/>
-      <c r="H24" s="6" t="inlineStr"/>
-      <c r="I24" s="6" t="inlineStr"/>
-      <c r="J24" s="6" t="inlineStr"/>
-      <c r="K24" s="6" t="inlineStr"/>
+      <c r="E24" s="10" t="inlineStr"/>
+      <c r="F24" s="10" t="inlineStr"/>
+      <c r="G24" s="10" t="inlineStr"/>
+      <c r="H24" s="10" t="inlineStr"/>
+      <c r="I24" s="10" t="inlineStr"/>
+      <c r="J24" s="10" t="inlineStr"/>
+      <c r="K24" s="10" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="inlineStr">
+      <c r="A25" s="21" t="inlineStr">
         <is>
           <t>Planning</t>
         </is>
       </c>
-      <c r="B25" s="7" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr">
         <is>
           <t>PLANNING_MX</t>
         </is>
       </c>
-      <c r="C25" s="12" t="n">
+      <c r="C25" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D25" s="7" t="inlineStr">
+      <c r="D25" s="21" t="inlineStr">
         <is>
           <t>All Planning phase tasks (IDP Solution Design, Data Flow Design, Security Architecture, Project Planning)</t>
         </is>
       </c>
-      <c r="E25" s="7" t="inlineStr"/>
-      <c r="F25" s="7" t="inlineStr"/>
-      <c r="G25" s="7" t="inlineStr"/>
-      <c r="H25" s="7" t="inlineStr"/>
-      <c r="I25" s="7" t="inlineStr"/>
-      <c r="J25" s="7" t="inlineStr"/>
-      <c r="K25" s="7" t="inlineStr"/>
+      <c r="E25" s="21" t="inlineStr"/>
+      <c r="F25" s="21" t="inlineStr"/>
+      <c r="G25" s="21" t="inlineStr"/>
+      <c r="H25" s="21" t="inlineStr"/>
+      <c r="I25" s="21" t="inlineStr"/>
+      <c r="J25" s="21" t="inlineStr"/>
+      <c r="K25" s="21" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="inlineStr">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B26" s="6" t="inlineStr">
+      <c r="B26" s="10" t="inlineStr">
         <is>
           <t>DEVELOPMENT_MX</t>
         </is>
       </c>
-      <c r="C26" s="12" t="n">
+      <c r="C26" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D26" s="6" t="inlineStr">
+      <c r="D26" s="10" t="inlineStr">
         <is>
           <t>All Development phase tasks (AWS Infrastructure, Document Pipeline, AI/ML Integration, Custom Models, API Development)</t>
         </is>
       </c>
-      <c r="E26" s="6" t="inlineStr"/>
-      <c r="F26" s="6" t="inlineStr"/>
-      <c r="G26" s="6" t="inlineStr"/>
-      <c r="H26" s="6" t="inlineStr"/>
-      <c r="I26" s="6" t="inlineStr"/>
-      <c r="J26" s="6" t="inlineStr"/>
-      <c r="K26" s="6" t="inlineStr"/>
+      <c r="E26" s="10" t="inlineStr"/>
+      <c r="F26" s="10" t="inlineStr"/>
+      <c r="G26" s="10" t="inlineStr"/>
+      <c r="H26" s="10" t="inlineStr"/>
+      <c r="I26" s="10" t="inlineStr"/>
+      <c r="J26" s="10" t="inlineStr"/>
+      <c r="K26" s="10" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="inlineStr">
+      <c r="A27" s="21" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B27" s="7" t="inlineStr">
+      <c r="B27" s="21" t="inlineStr">
         <is>
           <t>TESTING_MX</t>
         </is>
       </c>
-      <c r="C27" s="12" t="n">
+      <c r="C27" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D27" s="7" t="inlineStr">
+      <c r="D27" s="21" t="inlineStr">
         <is>
           <t>All Testing phase tasks (Unit Testing, Document Testing, Performance Testing, Accuracy Testing, Security Testing)</t>
         </is>
       </c>
-      <c r="E27" s="7" t="inlineStr"/>
-      <c r="F27" s="7" t="inlineStr"/>
-      <c r="G27" s="7" t="inlineStr"/>
-      <c r="H27" s="7" t="inlineStr"/>
-      <c r="I27" s="7" t="inlineStr"/>
-      <c r="J27" s="7" t="inlineStr"/>
-      <c r="K27" s="7" t="inlineStr"/>
+      <c r="E27" s="21" t="inlineStr"/>
+      <c r="F27" s="21" t="inlineStr"/>
+      <c r="G27" s="21" t="inlineStr"/>
+      <c r="H27" s="21" t="inlineStr"/>
+      <c r="I27" s="21" t="inlineStr"/>
+      <c r="J27" s="21" t="inlineStr"/>
+      <c r="K27" s="21" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="inlineStr">
+      <c r="A28" s="10" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="B28" s="6" t="inlineStr">
+      <c r="B28" s="10" t="inlineStr">
         <is>
           <t>DEPLOYMENT_MX</t>
         </is>
       </c>
-      <c r="C28" s="12" t="n">
+      <c r="C28" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="inlineStr">
+      <c r="D28" s="10" t="inlineStr">
         <is>
           <t>All Deployment phase tasks (Production Deployment, Model Deployment, Go-Live Support)</t>
         </is>
       </c>
-      <c r="E28" s="6" t="inlineStr"/>
-      <c r="F28" s="6" t="inlineStr"/>
-      <c r="G28" s="6" t="inlineStr"/>
-      <c r="H28" s="6" t="inlineStr"/>
-      <c r="I28" s="6" t="inlineStr"/>
-      <c r="J28" s="6" t="inlineStr"/>
-      <c r="K28" s="6" t="inlineStr"/>
+      <c r="E28" s="10" t="inlineStr"/>
+      <c r="F28" s="10" t="inlineStr"/>
+      <c r="G28" s="10" t="inlineStr"/>
+      <c r="H28" s="10" t="inlineStr"/>
+      <c r="I28" s="10" t="inlineStr"/>
+      <c r="J28" s="10" t="inlineStr"/>
+      <c r="K28" s="10" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="inlineStr">
+      <c r="A29" s="21" t="inlineStr">
         <is>
           <t>Training</t>
         </is>
       </c>
-      <c r="B29" s="7" t="inlineStr">
+      <c r="B29" s="21" t="inlineStr">
         <is>
           <t>TRAINING_MX</t>
         </is>
       </c>
-      <c r="C29" s="12" t="n">
+      <c r="C29" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D29" s="7" t="inlineStr">
+      <c r="D29" s="21" t="inlineStr">
         <is>
           <t>All Training phase tasks (Administrator Training, Business User Training, Documentation)</t>
         </is>
       </c>
-      <c r="E29" s="7" t="inlineStr"/>
-      <c r="F29" s="7" t="inlineStr"/>
-      <c r="G29" s="7" t="inlineStr"/>
-      <c r="H29" s="7" t="inlineStr"/>
-      <c r="I29" s="7" t="inlineStr"/>
-      <c r="J29" s="7" t="inlineStr"/>
-      <c r="K29" s="7" t="inlineStr"/>
+      <c r="E29" s="21" t="inlineStr"/>
+      <c r="F29" s="21" t="inlineStr"/>
+      <c r="G29" s="21" t="inlineStr"/>
+      <c r="H29" s="21" t="inlineStr"/>
+      <c r="I29" s="21" t="inlineStr"/>
+      <c r="J29" s="21" t="inlineStr"/>
+      <c r="K29" s="21" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="inlineStr">
+      <c r="A30" s="10" t="inlineStr">
         <is>
           <t>Closeout</t>
         </is>
       </c>
-      <c r="B30" s="6" t="inlineStr">
+      <c r="B30" s="10" t="inlineStr">
         <is>
           <t>CLOSEOUT_MX</t>
         </is>
       </c>
-      <c r="C30" s="12" t="n">
+      <c r="C30" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D30" s="6" t="inlineStr">
+      <c r="D30" s="10" t="inlineStr">
         <is>
           <t>All Closeout phase tasks (Knowledge Transfer, Performance Baseline)</t>
         </is>
       </c>
-      <c r="E30" s="6" t="inlineStr"/>
-      <c r="F30" s="6" t="inlineStr"/>
-      <c r="G30" s="6" t="inlineStr"/>
-      <c r="H30" s="6" t="inlineStr"/>
-      <c r="I30" s="6" t="inlineStr"/>
-      <c r="J30" s="6" t="inlineStr"/>
-      <c r="K30" s="6" t="inlineStr"/>
+      <c r="E30" s="10" t="inlineStr"/>
+      <c r="F30" s="10" t="inlineStr"/>
+      <c r="G30" s="10" t="inlineStr"/>
+      <c r="H30" s="10" t="inlineStr"/>
+      <c r="I30" s="10" t="inlineStr"/>
+      <c r="J30" s="10" t="inlineStr"/>
+      <c r="K30" s="10" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="inlineStr">
+      <c r="A31" s="21" t="inlineStr">
         <is>
           <t>Management</t>
         </is>
       </c>
-      <c r="B31" s="7" t="inlineStr">
+      <c r="B31" s="21" t="inlineStr">
         <is>
           <t>MANAGEMENT_MX</t>
         </is>
       </c>
-      <c r="C31" s="12" t="n">
+      <c r="C31" s="26" t="n">
         <v>1.5</v>
       </c>
-      <c r="D31" s="7" t="inlineStr">
+      <c r="D31" s="21" t="inlineStr">
         <is>
           <t>Project Management overhead - 10% of actual engineering hours</t>
         </is>
       </c>
-      <c r="E31" s="7" t="inlineStr"/>
-      <c r="F31" s="7" t="inlineStr"/>
-      <c r="G31" s="7" t="inlineStr"/>
-      <c r="H31" s="7" t="inlineStr"/>
-      <c r="I31" s="7" t="inlineStr"/>
-      <c r="J31" s="7" t="inlineStr"/>
-      <c r="K31" s="7" t="inlineStr"/>
+      <c r="E31" s="21" t="inlineStr"/>
+      <c r="F31" s="21" t="inlineStr"/>
+      <c r="G31" s="21" t="inlineStr"/>
+      <c r="H31" s="21" t="inlineStr"/>
+      <c r="I31" s="21" t="inlineStr"/>
+      <c r="J31" s="21" t="inlineStr"/>
+      <c r="K31" s="21" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="inlineStr">
+      <c r="A32" s="10" t="inlineStr">
         <is>
           <t>Leadership</t>
         </is>
       </c>
-      <c r="B32" s="6" t="inlineStr">
+      <c r="B32" s="10" t="inlineStr">
         <is>
           <t>LEADERSHIP_MX</t>
         </is>
       </c>
-      <c r="C32" s="12" t="n">
+      <c r="C32" s="26" t="n">
         <v>1.5</v>
       </c>
-      <c r="D32" s="6" t="inlineStr">
+      <c r="D32" s="10" t="inlineStr">
         <is>
           <t>Quarterback/Technical Leadership overhead - 10% of actual engineering hours</t>
         </is>
       </c>
-      <c r="E32" s="6" t="inlineStr"/>
-      <c r="F32" s="6" t="inlineStr"/>
-      <c r="G32" s="6" t="inlineStr"/>
-      <c r="H32" s="6" t="inlineStr"/>
-      <c r="I32" s="6" t="inlineStr"/>
-      <c r="J32" s="6" t="inlineStr"/>
-      <c r="K32" s="6" t="inlineStr"/>
+      <c r="E32" s="10" t="inlineStr"/>
+      <c r="F32" s="10" t="inlineStr"/>
+      <c r="G32" s="10" t="inlineStr"/>
+      <c r="H32" s="10" t="inlineStr"/>
+      <c r="I32" s="10" t="inlineStr"/>
+      <c r="J32" s="10" t="inlineStr"/>
+      <c r="K32" s="10" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="inlineStr"/>
-      <c r="B33" s="7" t="inlineStr"/>
-      <c r="C33" s="12" t="inlineStr"/>
-      <c r="D33" s="7" t="inlineStr"/>
-      <c r="E33" s="7" t="inlineStr"/>
-      <c r="F33" s="7" t="inlineStr"/>
-      <c r="G33" s="7" t="inlineStr"/>
-      <c r="H33" s="7" t="inlineStr"/>
-      <c r="I33" s="7" t="inlineStr"/>
-      <c r="J33" s="7" t="inlineStr"/>
-      <c r="K33" s="7" t="inlineStr"/>
+      <c r="A33" s="21" t="inlineStr"/>
+      <c r="B33" s="21" t="inlineStr"/>
+      <c r="C33" s="26" t="inlineStr"/>
+      <c r="D33" s="21" t="inlineStr"/>
+      <c r="E33" s="21" t="inlineStr"/>
+      <c r="F33" s="21" t="inlineStr"/>
+      <c r="G33" s="21" t="inlineStr"/>
+      <c r="H33" s="21" t="inlineStr"/>
+      <c r="I33" s="21" t="inlineStr"/>
+      <c r="J33" s="21" t="inlineStr"/>
+      <c r="K33" s="21" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1826,1566 +2034,1566 @@
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="19" t="inlineStr">
         <is>
           <t>Phase</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="19" t="inlineStr">
         <is>
           <t>Work Package</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="19" t="inlineStr">
         <is>
           <t>Task Description</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="19" t="inlineStr">
         <is>
           <t>Resource Type</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="19" t="inlineStr">
         <is>
           <t>Base Hours</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="19" t="inlineStr">
         <is>
           <t>Effort Multiplier</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="19" t="inlineStr">
         <is>
           <t>Actual Hours</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="19" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="19" t="inlineStr">
         <is>
           <t>Cost Estimate</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="19" t="inlineStr">
         <is>
           <t>Dependencies</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="19" t="inlineStr">
         <is>
           <t>Notes</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="10" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B2" s="10" t="inlineStr">
         <is>
           <t>Requirements Gathering</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
+      <c r="C2" s="10" t="inlineStr">
         <is>
           <t>Conduct stakeholder interviews for IDP requirements</t>
         </is>
       </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="D2" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="27" t="n">
         <v>32</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="28">
         <f>'Estimate Settings'!$C$24</f>
         <v/>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="10">
         <f>$E2*$F2</f>
         <v/>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="29" t="n">
         <v>150</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="10">
         <f>TEXT($G2*$H2,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J2" s="6" t="inlineStr"/>
-      <c r="K2" s="6" t="inlineStr">
+      <c r="J2" s="10" t="inlineStr"/>
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>Includes requirements documentation and document processing workflow analysis</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="21" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="B3" s="7" t="inlineStr">
+      <c r="B3" s="21" t="inlineStr">
         <is>
           <t>Document Analysis</t>
         </is>
       </c>
-      <c r="C3" s="7" t="inlineStr">
+      <c r="C3" s="21" t="inlineStr">
         <is>
           <t>Analyze document types volumes and data extraction requirements</t>
         </is>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E3" s="16" t="n">
+      <c r="E3" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="28">
         <f>'Estimate Settings'!$C$24</f>
         <v/>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="21">
         <f>$E3*$F3</f>
         <v/>
       </c>
-      <c r="H3" s="17" t="n">
+      <c r="H3" s="31" t="n">
         <v>200</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="21">
         <f>TEXT($G3*$H3,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J3" s="7" t="inlineStr"/>
-      <c r="K3" s="7" t="inlineStr">
+      <c r="J3" s="21" t="inlineStr"/>
+      <c r="K3" s="21" t="inlineStr">
         <is>
           <t>Customer must provide representative document samples for each document type</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="10" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="10" t="inlineStr">
         <is>
           <t>AWS Environment Assessment</t>
         </is>
       </c>
-      <c r="C4" s="6" t="inlineStr">
+      <c r="C4" s="10" t="inlineStr">
         <is>
           <t>Evaluate AWS infrastructure and AI/ML services readiness</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
+      <c r="D4" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="28">
         <f>'Estimate Settings'!$C$24</f>
         <v/>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="10">
         <f>$E4*$F4</f>
         <v/>
       </c>
-      <c r="H4" s="15" t="n">
+      <c r="H4" s="29" t="n">
         <v>200</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="10">
         <f>TEXT($G4*$H4,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J4" s="6" t="inlineStr"/>
-      <c r="K4" s="6" t="inlineStr">
+      <c r="J4" s="10" t="inlineStr"/>
+      <c r="K4" s="10" t="inlineStr">
         <is>
           <t>Customer must provide AWS account access and service limits information</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="21" t="inlineStr">
         <is>
           <t>Discovery</t>
         </is>
       </c>
-      <c r="B5" s="7" t="inlineStr">
+      <c r="B5" s="21" t="inlineStr">
         <is>
           <t>Compliance Review</t>
         </is>
       </c>
-      <c r="C5" s="7" t="inlineStr">
+      <c r="C5" s="21" t="inlineStr">
         <is>
           <t>Assess data privacy compliance and security requirements</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E5" s="16" t="n">
+      <c r="E5" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="28">
         <f>'Estimate Settings'!$C$24</f>
         <v/>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="21">
         <f>$E5*$F5</f>
         <v/>
       </c>
-      <c r="H5" s="17" t="n">
+      <c r="H5" s="31" t="n">
         <v>175</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="21">
         <f>TEXT($G5*$H5,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J5" s="7" t="inlineStr"/>
-      <c r="K5" s="7" t="inlineStr">
+      <c r="J5" s="21" t="inlineStr"/>
+      <c r="K5" s="21" t="inlineStr">
         <is>
           <t>Identifies PII/PHI handling requirements and document retention policies</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="10" t="inlineStr">
         <is>
           <t>Planning</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
+      <c r="B6" s="10" t="inlineStr">
         <is>
           <t>IDP Solution Design</t>
         </is>
       </c>
-      <c r="C6" s="6" t="inlineStr">
+      <c r="C6" s="10" t="inlineStr">
         <is>
           <t>Design AWS AI/ML architecture with Textract Comprehend A2I</t>
         </is>
       </c>
-      <c r="D6" s="6" t="inlineStr">
+      <c r="D6" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E6" s="13" t="n">
+      <c r="E6" s="27" t="n">
         <v>40</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="28">
         <f>'Estimate Settings'!$C$25</f>
         <v/>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="10">
         <f>$E6*$F6</f>
         <v/>
       </c>
-      <c r="H6" s="15" t="n">
+      <c r="H6" s="29" t="n">
         <v>200</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="10">
         <f>TEXT($G6*$H6,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J6" s="6" t="inlineStr">
+      <c r="J6" s="10" t="inlineStr">
         <is>
           <t>Requirements Gathering</t>
         </is>
       </c>
-      <c r="K6" s="6" t="inlineStr">
+      <c r="K6" s="10" t="inlineStr">
         <is>
           <t>Deliverable: AWS architecture diagram with AI/ML service integration design</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="inlineStr">
+      <c r="A7" s="21" t="inlineStr">
         <is>
           <t>Planning</t>
         </is>
       </c>
-      <c r="B7" s="7" t="inlineStr">
+      <c r="B7" s="21" t="inlineStr">
         <is>
           <t>Data Flow Design</t>
         </is>
       </c>
-      <c r="C7" s="7" t="inlineStr">
+      <c r="C7" s="21" t="inlineStr">
         <is>
           <t>Design document ingestion processing and output workflows</t>
         </is>
       </c>
-      <c r="D7" s="7" t="inlineStr">
+      <c r="D7" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E7" s="16" t="n">
+      <c r="E7" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="28">
         <f>'Estimate Settings'!$C$25</f>
         <v/>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="21">
         <f>$E7*$F7</f>
         <v/>
       </c>
-      <c r="H7" s="17" t="n">
+      <c r="H7" s="31" t="n">
         <v>180</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="21">
         <f>TEXT($G7*$H7,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J7" s="7" t="inlineStr">
+      <c r="J7" s="21" t="inlineStr">
         <is>
           <t>Document Analysis</t>
         </is>
       </c>
-      <c r="K7" s="7" t="inlineStr">
+      <c r="K7" s="21" t="inlineStr">
         <is>
           <t>Deliverable: Document processing workflow and data flow diagrams</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>Planning</t>
         </is>
       </c>
-      <c r="B8" s="6" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>Security Architecture</t>
         </is>
       </c>
-      <c r="C8" s="6" t="inlineStr">
+      <c r="C8" s="10" t="inlineStr">
         <is>
           <t>Design security controls encryption and access for documents</t>
         </is>
       </c>
-      <c r="D8" s="6" t="inlineStr">
+      <c r="D8" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="28">
         <f>'Estimate Settings'!$C$25</f>
         <v/>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="10">
         <f>$E8*$F8</f>
         <v/>
       </c>
-      <c r="H8" s="15" t="n">
+      <c r="H8" s="29" t="n">
         <v>175</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="10">
         <f>TEXT($G8*$H8,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J8" s="6" t="inlineStr">
+      <c r="J8" s="10" t="inlineStr">
         <is>
           <t>Compliance Review</t>
         </is>
       </c>
-      <c r="K8" s="6" t="inlineStr">
+      <c r="K8" s="10" t="inlineStr">
         <is>
           <t>Document encryption at rest/transit IAM roles and audit logging design</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="21" t="inlineStr">
         <is>
           <t>Planning</t>
         </is>
       </c>
-      <c r="B9" s="7" t="inlineStr">
+      <c r="B9" s="21" t="inlineStr">
         <is>
           <t>Project Planning</t>
         </is>
       </c>
-      <c r="C9" s="7" t="inlineStr">
+      <c r="C9" s="21" t="inlineStr">
         <is>
           <t>Develop implementation timeline and resource allocation</t>
         </is>
       </c>
-      <c r="D9" s="7" t="inlineStr">
+      <c r="D9" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E9" s="16" t="n">
+      <c r="E9" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="28">
         <f>'Estimate Settings'!$C$25</f>
         <v/>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="21">
         <f>$E9*$F9</f>
         <v/>
       </c>
-      <c r="H9" s="17" t="n">
+      <c r="H9" s="31" t="n">
         <v>140</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="21">
         <f>TEXT($G9*$H9,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J9" s="7" t="inlineStr">
+      <c r="J9" s="21" t="inlineStr">
         <is>
           <t>IDP Solution Design</t>
         </is>
       </c>
-      <c r="K9" s="7" t="inlineStr">
+      <c r="K9" s="21" t="inlineStr">
         <is>
           <t>Deliverable: Project plan with phased rollout and milestone schedule</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="6" t="inlineStr">
+      <c r="A10" s="10" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B10" s="6" t="inlineStr">
+      <c r="B10" s="10" t="inlineStr">
         <is>
           <t>AWS Infrastructure Setup</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C10" s="10" t="inlineStr">
         <is>
           <t>Provision Textract Comprehend S3 Lambda and supporting services</t>
         </is>
       </c>
-      <c r="D10" s="6" t="inlineStr">
+      <c r="D10" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="27" t="n">
         <v>40</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="10">
         <f>$E10*$F10</f>
         <v/>
       </c>
-      <c r="H10" s="15" t="n">
+      <c r="H10" s="29" t="n">
         <v>160</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="10">
         <f>TEXT($G10*$H10,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J10" s="6" t="inlineStr">
+      <c r="J10" s="10" t="inlineStr">
         <is>
           <t>IDP Solution Design</t>
         </is>
       </c>
-      <c r="K10" s="6" t="inlineStr">
+      <c r="K10" s="10" t="inlineStr">
         <is>
           <t>Includes S3 buckets Lambda functions API Gateway and CloudWatch setup</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="inlineStr">
+      <c r="A11" s="21" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B11" s="7" t="inlineStr">
+      <c r="B11" s="21" t="inlineStr">
         <is>
           <t>Document Processing Pipeline</t>
         </is>
       </c>
-      <c r="C11" s="7" t="inlineStr">
+      <c r="C11" s="21" t="inlineStr">
         <is>
           <t>Build document ingestion and processing workflows</t>
         </is>
       </c>
-      <c r="D11" s="7" t="inlineStr">
+      <c r="D11" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E11" s="16" t="n">
+      <c r="E11" s="30" t="n">
         <v>64</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="21">
         <f>$E11*$F11</f>
         <v/>
       </c>
-      <c r="H11" s="17" t="n">
+      <c r="H11" s="31" t="n">
         <v>130</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="21">
         <f>TEXT($G11*$H11,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J11" s="7" t="inlineStr">
+      <c r="J11" s="21" t="inlineStr">
         <is>
           <t>AWS Infrastructure Setup</t>
         </is>
       </c>
-      <c r="K11" s="7" t="inlineStr">
+      <c r="K11" s="21" t="inlineStr">
         <is>
           <t>Serverless event-driven pipeline with error handling and retry logic</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="6" t="inlineStr">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" s="10" t="inlineStr">
         <is>
           <t>AI/ML Model Integration</t>
         </is>
       </c>
-      <c r="C12" s="6" t="inlineStr">
+      <c r="C12" s="10" t="inlineStr">
         <is>
           <t>Integrate AWS Textract Comprehend and A2I services</t>
         </is>
       </c>
-      <c r="D12" s="6" t="inlineStr">
+      <c r="D12" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E12" s="13" t="n">
+      <c r="E12" s="27" t="n">
         <v>48</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="10">
         <f>$E12*$F12</f>
         <v/>
       </c>
-      <c r="H12" s="15" t="n">
+      <c r="H12" s="29" t="n">
         <v>170</v>
       </c>
-      <c r="I12" s="6">
+      <c r="I12" s="10">
         <f>TEXT($G12*$H12,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J12" s="6" t="inlineStr">
+      <c r="J12" s="10" t="inlineStr">
         <is>
           <t>Document Processing Pipeline</t>
         </is>
       </c>
-      <c r="K12" s="6" t="inlineStr">
+      <c r="K12" s="10" t="inlineStr">
         <is>
           <t>Configure Textract APIs Comprehend entity recognition and A2I workflows</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="A13" s="21" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B13" s="7" t="inlineStr">
+      <c r="B13" s="21" t="inlineStr">
         <is>
           <t>Custom Classification Models</t>
         </is>
       </c>
-      <c r="C13" s="7" t="inlineStr">
+      <c r="C13" s="21" t="inlineStr">
         <is>
           <t>Develop minimal classification logic for 2-3 document types</t>
         </is>
       </c>
-      <c r="D13" s="7" t="inlineStr">
+      <c r="D13" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E13" s="16" t="n">
+      <c r="E13" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="21">
         <f>$E13*$F13</f>
         <v/>
       </c>
-      <c r="H13" s="17" t="n">
+      <c r="H13" s="31" t="n">
         <v>165</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="21">
         <f>TEXT($G13*$H13,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J13" s="7" t="inlineStr">
+      <c r="J13" s="21" t="inlineStr">
         <is>
           <t>AI/ML Model Integration</t>
         </is>
       </c>
-      <c r="K13" s="7" t="inlineStr">
+      <c r="K13" s="21" t="inlineStr">
         <is>
           <t>Simple classification using AWS pre-built services - not full custom ML models</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="inlineStr">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B14" s="6" t="inlineStr">
+      <c r="B14" s="10" t="inlineStr">
         <is>
           <t>Data Extraction Logic</t>
         </is>
       </c>
-      <c r="C14" s="6" t="inlineStr">
+      <c r="C14" s="10" t="inlineStr">
         <is>
           <t>Build structured data extraction and validation logic</t>
         </is>
       </c>
-      <c r="D14" s="6" t="inlineStr">
+      <c r="D14" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E14" s="13" t="n">
+      <c r="E14" s="27" t="n">
         <v>32</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="10">
         <f>$E14*$F14</f>
         <v/>
       </c>
-      <c r="H14" s="15" t="n">
+      <c r="H14" s="29" t="n">
         <v>130</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="10">
         <f>TEXT($G14*$H14,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J14" s="6" t="inlineStr">
+      <c r="J14" s="10" t="inlineStr">
         <is>
           <t>Custom Classification Models</t>
         </is>
       </c>
-      <c r="K14" s="6" t="inlineStr">
+      <c r="K14" s="10" t="inlineStr">
         <is>
           <t>Includes field validation business rules and confidence scoring</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="inlineStr">
+      <c r="A15" s="21" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B15" s="7" t="inlineStr">
+      <c r="B15" s="21" t="inlineStr">
         <is>
           <t>API Development</t>
         </is>
       </c>
-      <c r="C15" s="7" t="inlineStr">
+      <c r="C15" s="21" t="inlineStr">
         <is>
           <t>Create REST APIs for document submission and retrieval</t>
         </is>
       </c>
-      <c r="D15" s="7" t="inlineStr">
+      <c r="D15" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E15" s="16" t="n">
+      <c r="E15" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="21">
         <f>$E15*$F15</f>
         <v/>
       </c>
-      <c r="H15" s="17" t="n">
+      <c r="H15" s="31" t="n">
         <v>125</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="21">
         <f>TEXT($G15*$H15,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J15" s="7" t="inlineStr">
+      <c r="J15" s="21" t="inlineStr">
         <is>
           <t>Data Extraction Logic</t>
         </is>
       </c>
-      <c r="K15" s="7" t="inlineStr">
+      <c r="K15" s="21" t="inlineStr">
         <is>
           <t>API Gateway endpoints with authentication and rate limiting</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="inlineStr">
+      <c r="A16" s="10" t="inlineStr">
         <is>
           <t>Development</t>
         </is>
       </c>
-      <c r="B16" s="6" t="inlineStr">
+      <c r="B16" s="10" t="inlineStr">
         <is>
           <t>Web Interface</t>
         </is>
       </c>
-      <c r="C16" s="6" t="inlineStr">
+      <c r="C16" s="10" t="inlineStr">
         <is>
           <t>Build document upload and results viewing interface</t>
         </is>
       </c>
-      <c r="D16" s="6" t="inlineStr">
+      <c r="D16" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E16" s="13" t="n">
+      <c r="E16" s="27" t="n">
         <v>32</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="28">
         <f>'Estimate Settings'!$C$26</f>
         <v/>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="10">
         <f>$E16*$F16</f>
         <v/>
       </c>
-      <c r="H16" s="15" t="n">
+      <c r="H16" s="29" t="n">
         <v>125</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="10">
         <f>TEXT($G16*$H16,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J16" s="6" t="inlineStr">
+      <c r="J16" s="10" t="inlineStr">
         <is>
           <t>API Development</t>
         </is>
       </c>
-      <c r="K16" s="6" t="inlineStr">
+      <c r="K16" s="10" t="inlineStr">
         <is>
           <t>Simple upload UI with drag-drop and results dashboard - not full application</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="inlineStr">
+      <c r="A17" s="21" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B17" s="7" t="inlineStr">
+      <c r="B17" s="21" t="inlineStr">
         <is>
           <t>Unit Testing</t>
         </is>
       </c>
-      <c r="C17" s="7" t="inlineStr">
+      <c r="C17" s="21" t="inlineStr">
         <is>
           <t>Develop automated tests for all processing components</t>
         </is>
       </c>
-      <c r="D17" s="7" t="inlineStr">
+      <c r="D17" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E17" s="16" t="n">
+      <c r="E17" s="30" t="n">
         <v>32</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="28">
         <f>'Estimate Settings'!$C$27</f>
         <v/>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="21">
         <f>$E17*$F17</f>
         <v/>
       </c>
-      <c r="H17" s="17" t="n">
+      <c r="H17" s="31" t="n">
         <v>120</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="21">
         <f>TEXT($G17*$H17,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J17" s="7" t="inlineStr">
+      <c r="J17" s="21" t="inlineStr">
         <is>
           <t>Data Extraction Logic</t>
         </is>
       </c>
-      <c r="K17" s="7" t="inlineStr">
+      <c r="K17" s="21" t="inlineStr">
         <is>
           <t>Automated test suite for Lambda functions and API endpoints</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="inlineStr">
+      <c r="A18" s="10" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B18" s="6" t="inlineStr">
+      <c r="B18" s="10" t="inlineStr">
         <is>
           <t>Document Processing Testing</t>
         </is>
       </c>
-      <c r="C18" s="6" t="inlineStr">
+      <c r="C18" s="10" t="inlineStr">
         <is>
           <t>Test various document types formats and qualities</t>
         </is>
       </c>
-      <c r="D18" s="6" t="inlineStr">
+      <c r="D18" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E18" s="13" t="n">
+      <c r="E18" s="27" t="n">
         <v>32</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="28">
         <f>'Estimate Settings'!$C$27</f>
         <v/>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="10">
         <f>$E18*$F18</f>
         <v/>
       </c>
-      <c r="H18" s="15" t="n">
+      <c r="H18" s="29" t="n">
         <v>120</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="10">
         <f>TEXT($G18*$H18,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J18" s="6" t="inlineStr">
+      <c r="J18" s="10" t="inlineStr">
         <is>
           <t>Web Interface</t>
         </is>
       </c>
-      <c r="K18" s="6" t="inlineStr">
+      <c r="K18" s="10" t="inlineStr">
         <is>
           <t>Customer must provide comprehensive test document library with variations</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="inlineStr">
+      <c r="A19" s="21" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B19" s="7" t="inlineStr">
+      <c r="B19" s="21" t="inlineStr">
         <is>
           <t>Performance Testing</t>
         </is>
       </c>
-      <c r="C19" s="7" t="inlineStr">
+      <c r="C19" s="21" t="inlineStr">
         <is>
           <t>Test system performance with high document volumes</t>
         </is>
       </c>
-      <c r="D19" s="7" t="inlineStr">
+      <c r="D19" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E19" s="16" t="n">
+      <c r="E19" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="28">
         <f>'Estimate Settings'!$C$27</f>
         <v/>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="21">
         <f>$E19*$F19</f>
         <v/>
       </c>
-      <c r="H19" s="17" t="n">
+      <c r="H19" s="31" t="n">
         <v>140</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="21">
         <f>TEXT($G19*$H19,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J19" s="7" t="inlineStr">
+      <c r="J19" s="21" t="inlineStr">
         <is>
           <t>Document Processing Testing</t>
         </is>
       </c>
-      <c r="K19" s="7" t="inlineStr">
+      <c r="K19" s="21" t="inlineStr">
         <is>
           <t>Load testing with realistic document volumes and concurrent processing</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="6" t="inlineStr">
+      <c r="A20" s="10" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B20" s="6" t="inlineStr">
+      <c r="B20" s="10" t="inlineStr">
         <is>
           <t>Accuracy Testing</t>
         </is>
       </c>
-      <c r="C20" s="6" t="inlineStr">
+      <c r="C20" s="10" t="inlineStr">
         <is>
           <t>Validate AI/ML model accuracy and data extraction quality</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
+      <c r="D20" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E20" s="13" t="n">
+      <c r="E20" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="28">
         <f>'Estimate Settings'!$C$27</f>
         <v/>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="10">
         <f>$E20*$F20</f>
         <v/>
       </c>
-      <c r="H20" s="15" t="n">
+      <c r="H20" s="29" t="n">
         <v>170</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="10">
         <f>TEXT($G20*$H20,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J20" s="6" t="inlineStr">
+      <c r="J20" s="10" t="inlineStr">
         <is>
           <t>Performance Testing</t>
         </is>
       </c>
-      <c r="K20" s="6" t="inlineStr">
+      <c r="K20" s="10" t="inlineStr">
         <is>
           <t>Statistical validation of extraction accuracy against labeled test dataset</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="inlineStr">
+      <c r="A21" s="21" t="inlineStr">
         <is>
           <t>Testing</t>
         </is>
       </c>
-      <c r="B21" s="7" t="inlineStr">
+      <c r="B21" s="21" t="inlineStr">
         <is>
           <t>Security Testing</t>
         </is>
       </c>
-      <c r="C21" s="7" t="inlineStr">
+      <c r="C21" s="21" t="inlineStr">
         <is>
           <t>Perform security testing on document handling pipeline</t>
         </is>
       </c>
-      <c r="D21" s="7" t="inlineStr">
+      <c r="D21" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E21" s="16" t="n">
+      <c r="E21" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="28">
         <f>'Estimate Settings'!$C$27</f>
         <v/>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="21">
         <f>$E21*$F21</f>
         <v/>
       </c>
-      <c r="H21" s="17" t="n">
+      <c r="H21" s="31" t="n">
         <v>175</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="21">
         <f>TEXT($G21*$H21,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J21" s="7" t="inlineStr">
+      <c r="J21" s="21" t="inlineStr">
         <is>
           <t>Accuracy Testing</t>
         </is>
       </c>
-      <c r="K21" s="7" t="inlineStr">
+      <c r="K21" s="21" t="inlineStr">
         <is>
           <t>Includes IAM policy validation encryption testing and audit log verification</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="6" t="inlineStr">
+      <c r="A22" s="10" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="B22" s="6" t="inlineStr">
+      <c r="B22" s="10" t="inlineStr">
         <is>
           <t>Production Deployment</t>
         </is>
       </c>
-      <c r="C22" s="6" t="inlineStr">
+      <c r="C22" s="10" t="inlineStr">
         <is>
           <t>Deploy IDP solution to production AWS environment</t>
         </is>
       </c>
-      <c r="D22" s="6" t="inlineStr">
+      <c r="D22" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E22" s="13" t="n">
+      <c r="E22" s="27" t="n">
         <v>24</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="28">
         <f>'Estimate Settings'!$C$28</f>
         <v/>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="10">
         <f>$E22*$F22</f>
         <v/>
       </c>
-      <c r="H22" s="15" t="n">
+      <c r="H22" s="29" t="n">
         <v>160</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="10">
         <f>TEXT($G22*$H22,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J22" s="6" t="inlineStr">
+      <c r="J22" s="10" t="inlineStr">
         <is>
           <t>Security Testing</t>
         </is>
       </c>
-      <c r="K22" s="6" t="inlineStr">
+      <c r="K22" s="10" t="inlineStr">
         <is>
           <t>Blue-green deployment with rollback procedures and smoke testing</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="inlineStr">
+      <c r="A23" s="21" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="B23" s="7" t="inlineStr">
+      <c r="B23" s="21" t="inlineStr">
         <is>
           <t>Model Deployment</t>
         </is>
       </c>
-      <c r="C23" s="7" t="inlineStr">
+      <c r="C23" s="21" t="inlineStr">
         <is>
           <t>Deploy trained ML models to production endpoints</t>
         </is>
       </c>
-      <c r="D23" s="7" t="inlineStr">
+      <c r="D23" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E23" s="16" t="n">
+      <c r="E23" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="28">
         <f>'Estimate Settings'!$C$28</f>
         <v/>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="21">
         <f>$E23*$F23</f>
         <v/>
       </c>
-      <c r="H23" s="17" t="n">
+      <c r="H23" s="31" t="n">
         <v>170</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="21">
         <f>TEXT($G23*$H23,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J23" s="7" t="inlineStr">
+      <c r="J23" s="21" t="inlineStr">
         <is>
           <t>Production Deployment</t>
         </is>
       </c>
-      <c r="K23" s="7" t="inlineStr">
+      <c r="K23" s="21" t="inlineStr">
         <is>
           <t>Deploy classification logic and configure production Textract/Comprehend</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="inlineStr">
+      <c r="A24" s="10" t="inlineStr">
         <is>
           <t>Deployment</t>
         </is>
       </c>
-      <c r="B24" s="6" t="inlineStr">
+      <c r="B24" s="10" t="inlineStr">
         <is>
           <t>Go-Live Support</t>
         </is>
       </c>
-      <c r="C24" s="6" t="inlineStr">
+      <c r="C24" s="10" t="inlineStr">
         <is>
           <t>Provide support during initial production rollout</t>
         </is>
       </c>
-      <c r="D24" s="6" t="inlineStr">
+      <c r="D24" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E24" s="13" t="n">
+      <c r="E24" s="27" t="n">
         <v>40</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="28">
         <f>'Estimate Settings'!$C$28</f>
         <v/>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="10">
         <f>$E24*$F24</f>
         <v/>
       </c>
-      <c r="H24" s="15" t="n">
+      <c r="H24" s="29" t="n">
         <v>110</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="10">
         <f>TEXT($G24*$H24,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J24" s="6" t="inlineStr">
+      <c r="J24" s="10" t="inlineStr">
         <is>
           <t>Model Deployment</t>
         </is>
       </c>
-      <c r="K24" s="6" t="inlineStr">
+      <c r="K24" s="10" t="inlineStr">
         <is>
           <t>Daily monitoring rapid issue response and accuracy validation during hypercare</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="inlineStr">
+      <c r="A25" s="21" t="inlineStr">
         <is>
           <t>Training</t>
         </is>
       </c>
-      <c r="B25" s="7" t="inlineStr">
+      <c r="B25" s="21" t="inlineStr">
         <is>
           <t>Administrator Training</t>
         </is>
       </c>
-      <c r="C25" s="7" t="inlineStr">
+      <c r="C25" s="21" t="inlineStr">
         <is>
           <t>Train system administrators on IDP solution management</t>
         </is>
       </c>
-      <c r="D25" s="7" t="inlineStr">
+      <c r="D25" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E25" s="16" t="n">
+      <c r="E25" s="30" t="n">
         <v>16</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="28">
         <f>'Estimate Settings'!$C$29</f>
         <v/>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="21">
         <f>$E25*$F25</f>
         <v/>
       </c>
-      <c r="H25" s="17" t="n">
+      <c r="H25" s="31" t="n">
         <v>130</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="21">
         <f>TEXT($G25*$H25,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J25" s="7" t="inlineStr">
+      <c r="J25" s="21" t="inlineStr">
         <is>
           <t>Production Deployment</t>
         </is>
       </c>
-      <c r="K25" s="7" t="inlineStr">
+      <c r="K25" s="21" t="inlineStr">
         <is>
           <t>Includes AWS service management CloudWatch monitoring and troubleshooting</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="6" t="inlineStr">
+      <c r="A26" s="10" t="inlineStr">
         <is>
           <t>Training</t>
         </is>
       </c>
-      <c r="B26" s="6" t="inlineStr">
+      <c r="B26" s="10" t="inlineStr">
         <is>
           <t>Business User Training</t>
         </is>
       </c>
-      <c r="C26" s="6" t="inlineStr">
+      <c r="C26" s="10" t="inlineStr">
         <is>
           <t>Train users on document submission and results review</t>
         </is>
       </c>
-      <c r="D26" s="6" t="inlineStr">
+      <c r="D26" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E26" s="13" t="n">
+      <c r="E26" s="27" t="n">
         <v>16</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="28">
         <f>'Estimate Settings'!$C$29</f>
         <v/>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="10">
         <f>$E26*$F26</f>
         <v/>
       </c>
-      <c r="H26" s="15" t="n">
+      <c r="H26" s="29" t="n">
         <v>120</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="10">
         <f>TEXT($G26*$H26,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J26" s="6" t="inlineStr">
+      <c r="J26" s="10" t="inlineStr">
         <is>
           <t>Administrator Training</t>
         </is>
       </c>
-      <c r="K26" s="6" t="inlineStr">
+      <c r="K26" s="10" t="inlineStr">
         <is>
           <t>Role-based training for document processors and quality reviewers</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="inlineStr">
+      <c r="A27" s="21" t="inlineStr">
         <is>
           <t>Training</t>
         </is>
       </c>
-      <c r="B27" s="7" t="inlineStr">
+      <c r="B27" s="21" t="inlineStr">
         <is>
           <t>Documentation</t>
         </is>
       </c>
-      <c r="C27" s="7" t="inlineStr">
+      <c r="C27" s="21" t="inlineStr">
         <is>
           <t>Create user guides technical documentation and runbooks</t>
         </is>
       </c>
-      <c r="D27" s="7" t="inlineStr">
+      <c r="D27" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E27" s="16" t="n">
+      <c r="E27" s="30" t="n">
         <v>24</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="28">
         <f>'Estimate Settings'!$C$29</f>
         <v/>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="21">
         <f>$E27*$F27</f>
         <v/>
       </c>
-      <c r="H27" s="17" t="n">
+      <c r="H27" s="31" t="n">
         <v>110</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="21">
         <f>TEXT($G27*$H27,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J27" s="7" t="inlineStr">
+      <c r="J27" s="21" t="inlineStr">
         <is>
           <t>Business User Training</t>
         </is>
       </c>
-      <c r="K27" s="7" t="inlineStr">
+      <c r="K27" s="21" t="inlineStr">
         <is>
           <t>Deliverable: Operations runbook user guides and troubleshooting procedures</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="inlineStr">
+      <c r="A28" s="10" t="inlineStr">
         <is>
           <t>Closeout</t>
         </is>
       </c>
-      <c r="B28" s="6" t="inlineStr">
+      <c r="B28" s="10" t="inlineStr">
         <is>
           <t>Knowledge Transfer</t>
         </is>
       </c>
-      <c r="C28" s="6" t="inlineStr">
+      <c r="C28" s="10" t="inlineStr">
         <is>
           <t>Transfer solution ownership to client operations team</t>
         </is>
       </c>
-      <c r="D28" s="6" t="inlineStr">
+      <c r="D28" s="10" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E28" s="13" t="n">
+      <c r="E28" s="27" t="n">
         <v>16</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="28">
         <f>'Estimate Settings'!$C$30</f>
         <v/>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="10">
         <f>$E28*$F28</f>
         <v/>
       </c>
-      <c r="H28" s="15" t="n">
+      <c r="H28" s="29" t="n">
         <v>140</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="10">
         <f>TEXT($G28*$H28,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J28" s="6" t="inlineStr">
+      <c r="J28" s="10" t="inlineStr">
         <is>
           <t>Documentation</t>
         </is>
       </c>
-      <c r="K28" s="6" t="inlineStr">
+      <c r="K28" s="10" t="inlineStr">
         <is>
           <t>Comprehensive handover including AWS architecture model details and procedures</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="inlineStr">
+      <c r="A29" s="21" t="inlineStr">
         <is>
           <t>Closeout</t>
         </is>
       </c>
-      <c r="B29" s="7" t="inlineStr">
+      <c r="B29" s="21" t="inlineStr">
         <is>
           <t>Performance Baseline</t>
         </is>
       </c>
-      <c r="C29" s="7" t="inlineStr">
+      <c r="C29" s="21" t="inlineStr">
         <is>
           <t>Establish performance metrics and monitoring baselines</t>
         </is>
       </c>
-      <c r="D29" s="7" t="inlineStr">
+      <c r="D29" s="21" t="inlineStr">
         <is>
           <t>EO Engineer</t>
         </is>
       </c>
-      <c r="E29" s="16" t="n">
+      <c r="E29" s="30" t="n">
         <v>8</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="28">
         <f>'Estimate Settings'!$C$30</f>
         <v/>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="21">
         <f>$E29*$F29</f>
         <v/>
       </c>
-      <c r="H29" s="17" t="n">
+      <c r="H29" s="31" t="n">
         <v>130</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="21">
         <f>TEXT($G29*$H29,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J29" s="7" t="inlineStr">
+      <c r="J29" s="21" t="inlineStr">
         <is>
           <t>Knowledge Transfer</t>
         </is>
       </c>
-      <c r="K29" s="7" t="inlineStr">
+      <c r="K29" s="21" t="inlineStr">
         <is>
           <t>Establishes accuracy SLAs processing time metrics and cost monitoring</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="6" t="inlineStr">
+      <c r="A30" s="10" t="inlineStr">
         <is>
           <t>Management</t>
         </is>
       </c>
-      <c r="B30" s="6" t="inlineStr">
+      <c r="B30" s="10" t="inlineStr">
         <is>
           <t>Technical Leadership</t>
         </is>
       </c>
-      <c r="C30" s="6" t="inlineStr">
+      <c r="C30" s="10" t="inlineStr">
         <is>
           <t>Quarterback technical oversight and architecture review</t>
         </is>
       </c>
-      <c r="D30" s="6" t="inlineStr">
+      <c r="D30" s="10" t="inlineStr">
         <is>
           <t>EO Quarterback</t>
         </is>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="10">
         <f>ROUND(SUM($G$2:$G$29)*0.10,0)</f>
         <v/>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="28">
         <f>'Estimate Settings'!$C$32</f>
         <v/>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="10">
         <f>$E30*$F30</f>
         <v/>
       </c>
-      <c r="H30" s="15" t="n">
+      <c r="H30" s="29" t="n">
         <v>200</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="10">
         <f>TEXT($G30*$H30,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J30" s="6" t="inlineStr"/>
-      <c r="K30" s="6" t="inlineStr">
+      <c r="J30" s="10" t="inlineStr"/>
+      <c r="K30" s="10" t="inlineStr">
         <is>
           <t>AWS AI/ML architecture review and technical escalation support</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="inlineStr">
+      <c r="A31" s="21" t="inlineStr">
         <is>
           <t>Management</t>
         </is>
       </c>
-      <c r="B31" s="7" t="inlineStr">
+      <c r="B31" s="21" t="inlineStr">
         <is>
           <t>Project Management</t>
         </is>
       </c>
-      <c r="C31" s="7" t="inlineStr">
+      <c r="C31" s="21" t="inlineStr">
         <is>
           <t>Project coordination planning and management activities</t>
         </is>
       </c>
-      <c r="D31" s="7" t="inlineStr">
+      <c r="D31" s="21" t="inlineStr">
         <is>
           <t>EO Project Manager</t>
         </is>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="21">
         <f>ROUND(SUM($G$2:$G$29)*0.10,0)</f>
         <v/>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="28">
         <f>'Estimate Settings'!$C$31</f>
         <v/>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="21">
         <f>$E31*$F31</f>
         <v/>
       </c>
-      <c r="H31" s="17" t="n">
+      <c r="H31" s="31" t="n">
         <v>150</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="21">
         <f>TEXT($G31*$H31,"$#,##0")</f>
         <v/>
       </c>
-      <c r="J31" s="7" t="inlineStr"/>
-      <c r="K31" s="7" t="inlineStr">
+      <c r="J31" s="21" t="inlineStr"/>
+      <c r="K31" s="21" t="inlineStr">
         <is>
           <t>Includes weekly status reporting risk management and stakeholder coordination</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="inlineStr"/>
-      <c r="B32" s="6" t="inlineStr"/>
-      <c r="C32" s="6" t="inlineStr"/>
-      <c r="D32" s="6" t="inlineStr"/>
-      <c r="E32" s="13" t="inlineStr"/>
-      <c r="F32" s="14" t="inlineStr">
+      <c r="A32" s="28" t="inlineStr"/>
+      <c r="B32" s="28" t="inlineStr"/>
+      <c r="C32" s="28" t="inlineStr"/>
+      <c r="D32" s="28" t="inlineStr"/>
+      <c r="E32" s="32" t="inlineStr"/>
+      <c r="F32" s="16" t="inlineStr">
         <is>
           <t>TOTAL HOURS</t>
         </is>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="16">
         <f>SUM($G$2:$G$31)</f>
         <v/>
       </c>
-      <c r="H32" s="6" t="inlineStr">
+      <c r="H32" s="16" t="inlineStr">
         <is>
           <t>TOTAL COST</t>
         </is>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="16">
         <f>TEXT(SUMPRODUCT($G$2:$G$31,$H$2:$H$31),"$#,##0")</f>
         <v/>
       </c>
-      <c r="J32" s="6" t="inlineStr"/>
-      <c r="K32" s="6" t="inlineStr">
+      <c r="J32" s="28" t="inlineStr"/>
+      <c r="K32" s="16" t="inlineStr">
         <is>
           <t>EO Sales Engineer: Update phase-based multipliers in Estimate Settings based on customer document processing scope</t>
         </is>

</xml_diff>